<commit_message>
Replace ARMS Nut composition_edited_Sep_25 file
</commit_message>
<xml_diff>
--- a/NutritionComp/ARMS Nut composition_edited_Sep_25.xlsx
+++ b/NutritionComp/ARMS Nut composition_edited_Sep_25.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkelahan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkelahan/Desktop/Nutrient composition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B638008-1181-9A48-802D-117E5314D8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10F50E4-8575-A249-8D10-C5CAF72D2D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{0F6D54AC-2C38-EC4E-8BA4-DF77EF1E39DA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0F6D54AC-2C38-EC4E-8BA4-DF77EF1E39DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AF$159</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$A$159</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="330">
   <si>
     <t>Can</t>
   </si>
@@ -1081,7 +1087,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1100,8 +1106,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1124,12 +1136,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1168,6 +1193,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1503,11 +1534,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C02D22-C5E3-6846-A49B-8DFDD4C89904}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AF159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H161" sqref="H161"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1599,7 +1631,7 @@
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1659,7 @@
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1658,7 +1690,7 @@
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1689,7 +1721,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1726,7 +1758,7 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1754,7 +1786,7 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1814,7 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -1816,7 +1848,7 @@
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1882,7 @@
       <c r="AE9" s="3"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="10" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1890,7 +1922,7 @@
       <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
     </row>
-    <row r="11" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1918,7 +1950,7 @@
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
     </row>
-    <row r="12" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
@@ -1946,7 +1978,7 @@
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
     </row>
-    <row r="13" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +2006,7 @@
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
     </row>
-    <row r="14" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2034,7 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -2039,7 +2071,7 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -2067,7 +2099,7 @@
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
     </row>
-    <row r="17" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
@@ -2102,7 +2134,7 @@
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
     </row>
-    <row r="18" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -2133,7 +2165,7 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
@@ -2185,7 +2217,7 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
     </row>
-    <row r="20" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
@@ -2234,7 +2266,7 @@
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -2277,7 +2309,7 @@
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>30</v>
       </c>
@@ -2311,7 +2343,7 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
@@ -2339,7 +2371,7 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -2370,7 +2402,7 @@
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
@@ -2404,7 +2436,7 @@
       <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
     </row>
-    <row r="26" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>30</v>
       </c>
@@ -2432,7 +2464,7 @@
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
     </row>
-    <row r="27" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
@@ -2475,7 +2507,7 @@
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
     </row>
-    <row r="28" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -2506,7 +2538,7 @@
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
     </row>
-    <row r="29" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
@@ -2540,7 +2572,7 @@
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
     </row>
-    <row r="30" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>68</v>
       </c>
@@ -2574,7 +2606,7 @@
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
     </row>
-    <row r="31" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>64</v>
       </c>
@@ -2614,7 +2646,7 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
     </row>
-    <row r="32" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>64</v>
       </c>
@@ -2648,7 +2680,7 @@
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
     </row>
-    <row r="33" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>73</v>
       </c>
@@ -2679,7 +2711,7 @@
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
     </row>
-    <row r="34" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>68</v>
       </c>
@@ -2728,7 +2760,7 @@
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
     </row>
-    <row r="35" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>76</v>
       </c>
@@ -2759,7 +2791,7 @@
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
     </row>
-    <row r="36" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>76</v>
       </c>
@@ -2796,7 +2828,7 @@
       <c r="AE36" s="3"/>
       <c r="AF36" s="3"/>
     </row>
-    <row r="37" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
@@ -2839,7 +2871,7 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="3"/>
     </row>
-    <row r="38" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>64</v>
       </c>
@@ -2873,7 +2905,7 @@
       <c r="AE38" s="3"/>
       <c r="AF38" s="3"/>
     </row>
-    <row r="39" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>76</v>
       </c>
@@ -2901,7 +2933,7 @@
       <c r="AE39" s="3"/>
       <c r="AF39" s="3"/>
     </row>
-    <row r="40" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>64</v>
       </c>
@@ -2935,7 +2967,7 @@
       <c r="AE40" s="3"/>
       <c r="AF40" s="3"/>
     </row>
-    <row r="41" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>30</v>
       </c>
@@ -2966,7 +2998,7 @@
       <c r="AE41" s="3"/>
       <c r="AF41" s="3"/>
     </row>
-    <row r="42" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>73</v>
       </c>
@@ -3000,7 +3032,7 @@
       <c r="AE42" s="3"/>
       <c r="AF42" s="3"/>
     </row>
-    <row r="43" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>73</v>
       </c>
@@ -3031,7 +3063,7 @@
       <c r="AE43" s="3"/>
       <c r="AF43" s="3"/>
     </row>
-    <row r="44" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>30</v>
       </c>
@@ -3062,7 +3094,7 @@
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
     </row>
-    <row r="45" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3140,7 @@
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
     </row>
-    <row r="46" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>64</v>
       </c>
@@ -3160,7 +3192,7 @@
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
     </row>
-    <row r="47" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>95</v>
       </c>
@@ -3191,7 +3223,7 @@
       <c r="AE47" s="3"/>
       <c r="AF47" s="3"/>
     </row>
-    <row r="48" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>97</v>
       </c>
@@ -3219,7 +3251,7 @@
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
     </row>
-    <row r="49" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>97</v>
       </c>
@@ -3253,7 +3285,7 @@
       <c r="AE49" s="3"/>
       <c r="AF49" s="3"/>
     </row>
-    <row r="50" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>97</v>
       </c>
@@ -3284,7 +3316,7 @@
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
     </row>
-    <row r="51" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>97</v>
       </c>
@@ -3312,7 +3344,7 @@
       <c r="AE51" s="3"/>
       <c r="AF51" s="3"/>
     </row>
-    <row r="52" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>97</v>
       </c>
@@ -3343,7 +3375,7 @@
       <c r="AE52" s="3"/>
       <c r="AF52" s="3"/>
     </row>
-    <row r="53" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>97</v>
       </c>
@@ -3371,7 +3403,7 @@
       <c r="AE53" s="3"/>
       <c r="AF53" s="3"/>
     </row>
-    <row r="54" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>73</v>
       </c>
@@ -3405,7 +3437,7 @@
       <c r="AE54" s="3"/>
       <c r="AF54" s="3"/>
     </row>
-    <row r="55" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>73</v>
       </c>
@@ -3445,7 +3477,7 @@
       <c r="AE55" s="3"/>
       <c r="AF55" s="3"/>
     </row>
-    <row r="56" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>73</v>
       </c>
@@ -3476,7 +3508,7 @@
       <c r="AE56" s="3"/>
       <c r="AF56" s="3"/>
     </row>
-    <row r="57" spans="1:32" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:32" s="4" customFormat="1" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>73</v>
       </c>
@@ -3516,7 +3548,7 @@
       <c r="AE57" s="3"/>
       <c r="AF57" s="3"/>
     </row>
-    <row r="58" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>73</v>
       </c>
@@ -3547,7 +3579,7 @@
       <c r="AE58" s="3"/>
       <c r="AF58" s="3"/>
     </row>
-    <row r="59" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>97</v>
       </c>
@@ -3575,7 +3607,7 @@
       <c r="AE59" s="3"/>
       <c r="AF59" s="3"/>
     </row>
-    <row r="60" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>97</v>
       </c>
@@ -3609,7 +3641,7 @@
       <c r="AE60" s="3"/>
       <c r="AF60" s="3"/>
     </row>
-    <row r="61" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>97</v>
       </c>
@@ -3637,7 +3669,7 @@
       <c r="AE61" s="3"/>
       <c r="AF61" s="3"/>
     </row>
-    <row r="62" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>97</v>
       </c>
@@ -3668,7 +3700,7 @@
       <c r="AE62" s="3"/>
       <c r="AF62" s="3"/>
     </row>
-    <row r="63" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>97</v>
       </c>
@@ -3699,7 +3731,7 @@
       <c r="AE63" s="3"/>
       <c r="AF63" s="3"/>
     </row>
-    <row r="64" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>126</v>
       </c>
@@ -3736,7 +3768,7 @@
       <c r="AE64" s="3"/>
       <c r="AF64" s="3"/>
     </row>
-    <row r="65" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>126</v>
       </c>
@@ -3767,7 +3799,7 @@
       <c r="AE65" s="3"/>
       <c r="AF65" s="3"/>
     </row>
-    <row r="66" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>126</v>
       </c>
@@ -3795,7 +3827,7 @@
       <c r="AE66" s="3"/>
       <c r="AF66" s="3"/>
     </row>
-    <row r="67" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>126</v>
       </c>
@@ -3823,7 +3855,7 @@
       <c r="AE67" s="3"/>
       <c r="AF67" s="3"/>
     </row>
-    <row r="68" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>126</v>
       </c>
@@ -3851,7 +3883,7 @@
       <c r="AE68" s="3"/>
       <c r="AF68" s="3"/>
     </row>
-    <row r="69" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>126</v>
       </c>
@@ -3879,7 +3911,7 @@
       <c r="AE69" s="3"/>
       <c r="AF69" s="3"/>
     </row>
-    <row r="70" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>126</v>
       </c>
@@ -3913,7 +3945,7 @@
       <c r="AE70" s="3"/>
       <c r="AF70" s="3"/>
     </row>
-    <row r="71" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>126</v>
       </c>
@@ -3950,7 +3982,7 @@
       <c r="AE71" s="3"/>
       <c r="AF71" s="3"/>
     </row>
-    <row r="72" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>126</v>
       </c>
@@ -3978,7 +4010,7 @@
       <c r="AE72" s="3"/>
       <c r="AF72" s="3"/>
     </row>
-    <row r="73" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>126</v>
       </c>
@@ -4024,7 +4056,7 @@
       <c r="AE73" s="3"/>
       <c r="AF73" s="3"/>
     </row>
-    <row r="74" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>126</v>
       </c>
@@ -4058,7 +4090,7 @@
       <c r="AE74" s="3"/>
       <c r="AF74" s="3"/>
     </row>
-    <row r="75" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>126</v>
       </c>
@@ -4092,7 +4124,7 @@
       <c r="AE75" s="3"/>
       <c r="AF75" s="3"/>
     </row>
-    <row r="76" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>126</v>
       </c>
@@ -4132,7 +4164,7 @@
       <c r="AE76" s="3"/>
       <c r="AF76" s="3"/>
     </row>
-    <row r="77" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>126</v>
       </c>
@@ -4160,7 +4192,7 @@
       <c r="AE77" s="3"/>
       <c r="AF77" s="3"/>
     </row>
-    <row r="78" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>126</v>
       </c>
@@ -4188,7 +4220,7 @@
       <c r="AE78" s="3"/>
       <c r="AF78" s="3"/>
     </row>
-    <row r="79" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>126</v>
       </c>
@@ -4219,7 +4251,7 @@
       <c r="AE79" s="3"/>
       <c r="AF79" s="3"/>
     </row>
-    <row r="80" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>76</v>
       </c>
@@ -4256,7 +4288,7 @@
       <c r="AE80" s="3"/>
       <c r="AF80" s="3"/>
     </row>
-    <row r="81" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>161</v>
       </c>
@@ -4287,7 +4319,7 @@
       <c r="AE81" s="3"/>
       <c r="AF81" s="3"/>
     </row>
-    <row r="82" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>161</v>
       </c>
@@ -4318,7 +4350,7 @@
       <c r="AE82" s="3"/>
       <c r="AF82" s="3"/>
     </row>
-    <row r="83" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>76</v>
       </c>
@@ -4358,7 +4390,7 @@
       <c r="AE83" s="3"/>
       <c r="AF83" s="3"/>
     </row>
-    <row r="84" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>76</v>
       </c>
@@ -4420,7 +4452,7 @@
       <c r="AE85" s="3"/>
       <c r="AF85" s="3"/>
     </row>
-    <row r="86" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>76</v>
       </c>
@@ -4479,7 +4511,7 @@
       <c r="AE87" s="3"/>
       <c r="AF87" s="3"/>
     </row>
-    <row r="88" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>76</v>
       </c>
@@ -4507,7 +4539,7 @@
       <c r="AE88" s="3"/>
       <c r="AF88" s="3"/>
     </row>
-    <row r="89" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>76</v>
       </c>
@@ -4544,7 +4576,7 @@
       <c r="AE89" s="3"/>
       <c r="AF89" s="3"/>
     </row>
-    <row r="90" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>76</v>
       </c>
@@ -4575,7 +4607,7 @@
       <c r="AE90" s="3"/>
       <c r="AF90" s="3"/>
     </row>
-    <row r="91" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>76</v>
       </c>
@@ -4609,7 +4641,7 @@
       <c r="AE91" s="3"/>
       <c r="AF91" s="3"/>
     </row>
-    <row r="92" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>76</v>
       </c>
@@ -4643,7 +4675,7 @@
       <c r="AE92" s="3"/>
       <c r="AF92" s="3"/>
     </row>
-    <row r="93" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>76</v>
       </c>
@@ -4671,7 +4703,7 @@
       <c r="AE93" s="3"/>
       <c r="AF93" s="3"/>
     </row>
-    <row r="94" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>76</v>
       </c>
@@ -4705,7 +4737,7 @@
       <c r="AE94" s="3"/>
       <c r="AF94" s="3"/>
     </row>
-    <row r="95" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>161</v>
       </c>
@@ -4773,7 +4805,7 @@
       <c r="AE96" s="3"/>
       <c r="AF96" s="3"/>
     </row>
-    <row r="97" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>76</v>
       </c>
@@ -4810,7 +4842,7 @@
       <c r="AE97" s="3"/>
       <c r="AF97" s="3"/>
     </row>
-    <row r="98" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>76</v>
       </c>
@@ -4900,7 +4932,7 @@
       <c r="AE100" s="3"/>
       <c r="AF100" s="3"/>
     </row>
-    <row r="101" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>76</v>
       </c>
@@ -4931,7 +4963,7 @@
       <c r="AE101" s="3"/>
       <c r="AF101" s="3"/>
     </row>
-    <row r="102" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>76</v>
       </c>
@@ -4965,7 +4997,7 @@
       <c r="AE102" s="3"/>
       <c r="AF102" s="3"/>
     </row>
-    <row r="103" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>76</v>
       </c>
@@ -4993,7 +5025,7 @@
       <c r="AE103" s="3"/>
       <c r="AF103" s="3"/>
     </row>
-    <row r="104" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>76</v>
       </c>
@@ -5030,7 +5062,7 @@
       <c r="AE104" s="3"/>
       <c r="AF104" s="3"/>
     </row>
-    <row r="105" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>161</v>
       </c>
@@ -5092,7 +5124,7 @@
       <c r="AE106" s="3"/>
       <c r="AF106" s="3"/>
     </row>
-    <row r="107" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>76</v>
       </c>
@@ -5123,7 +5155,7 @@
       <c r="AE107" s="3"/>
       <c r="AF107" s="3"/>
     </row>
-    <row r="108" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>76</v>
       </c>
@@ -5151,7 +5183,7 @@
       <c r="AE108" s="3"/>
       <c r="AF108" s="3"/>
     </row>
-    <row r="109" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>76</v>
       </c>
@@ -5179,7 +5211,7 @@
       <c r="AE109" s="3"/>
       <c r="AF109" s="3"/>
     </row>
-    <row r="110" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>76</v>
       </c>
@@ -5210,7 +5242,7 @@
       <c r="AE110" s="3"/>
       <c r="AF110" s="3"/>
     </row>
-    <row r="111" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>76</v>
       </c>
@@ -5250,7 +5282,7 @@
       <c r="AE111" s="3"/>
       <c r="AF111" s="3"/>
     </row>
-    <row r="112" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>76</v>
       </c>
@@ -5284,7 +5316,7 @@
       <c r="AE112" s="3"/>
       <c r="AF112" s="3"/>
     </row>
-    <row r="113" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>223</v>
       </c>
@@ -5327,7 +5359,7 @@
       <c r="AE113" s="3"/>
       <c r="AF113" s="3"/>
     </row>
-    <row r="114" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>223</v>
       </c>
@@ -5355,7 +5387,7 @@
       <c r="AE114" s="3"/>
       <c r="AF114" s="3"/>
     </row>
-    <row r="115" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>223</v>
       </c>
@@ -5392,7 +5424,7 @@
       <c r="AE115" s="3"/>
       <c r="AF115" s="3"/>
     </row>
-    <row r="116" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>223</v>
       </c>
@@ -5432,7 +5464,7 @@
       <c r="AE116" s="3"/>
       <c r="AF116" s="3"/>
     </row>
-    <row r="117" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>223</v>
       </c>
@@ -5460,7 +5492,7 @@
       <c r="AE117" s="3"/>
       <c r="AF117" s="3"/>
     </row>
-    <row r="118" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>223</v>
       </c>
@@ -5491,7 +5523,7 @@
       <c r="AE118" s="3"/>
       <c r="AF118" s="3"/>
     </row>
-    <row r="119" spans="1:32" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:32" s="13" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
         <v>237</v>
       </c>
@@ -5516,7 +5548,7 @@
       <c r="AE119" s="3"/>
       <c r="AF119" s="3"/>
     </row>
-    <row r="120" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:32" s="13" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
         <v>237</v>
       </c>
@@ -5541,7 +5573,7 @@
       <c r="AE120" s="3"/>
       <c r="AF120" s="3"/>
     </row>
-    <row r="121" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:32" s="13" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
         <v>237</v>
       </c>
@@ -5566,7 +5598,7 @@
       <c r="AE121" s="3"/>
       <c r="AF121" s="3"/>
     </row>
-    <row r="122" spans="1:32" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:32" s="13" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
         <v>245</v>
       </c>
@@ -5594,7 +5626,7 @@
       <c r="AE122" s="3"/>
       <c r="AF122" s="3"/>
     </row>
-    <row r="123" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:32" s="13" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="s">
         <v>237</v>
       </c>
@@ -5619,7 +5651,7 @@
       <c r="AE123" s="3"/>
       <c r="AF123" s="3"/>
     </row>
-    <row r="124" spans="1:32" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:32" s="13" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
         <v>237</v>
       </c>
@@ -5644,7 +5676,7 @@
       <c r="AE124" s="3"/>
       <c r="AF124" s="3"/>
     </row>
-    <row r="125" spans="1:32" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:32" s="13" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
         <v>237</v>
       </c>
@@ -5669,7 +5701,7 @@
       <c r="AE125" s="3"/>
       <c r="AF125" s="3"/>
     </row>
-    <row r="126" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>64</v>
       </c>
@@ -5709,7 +5741,7 @@
       <c r="AE126" s="3"/>
       <c r="AF126" s="3"/>
     </row>
-    <row r="127" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>64</v>
       </c>
@@ -5743,7 +5775,7 @@
       <c r="AE127" s="3"/>
       <c r="AF127" s="3"/>
     </row>
-    <row r="128" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>64</v>
       </c>
@@ -5774,7 +5806,7 @@
       <c r="AE128" s="3"/>
       <c r="AF128" s="3"/>
     </row>
-    <row r="129" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>76</v>
       </c>
@@ -5805,7 +5837,7 @@
       <c r="AE129" s="3"/>
       <c r="AF129" s="3"/>
     </row>
-    <row r="130" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>64</v>
       </c>
@@ -5839,7 +5871,7 @@
       <c r="AE130" s="3"/>
       <c r="AF130" s="3"/>
     </row>
-    <row r="131" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>64</v>
       </c>
@@ -5873,7 +5905,7 @@
       <c r="AE131" s="3"/>
       <c r="AF131" s="3"/>
     </row>
-    <row r="132" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>64</v>
       </c>
@@ -5916,7 +5948,7 @@
       <c r="AE132" s="3"/>
       <c r="AF132" s="3"/>
     </row>
-    <row r="133" spans="1:32" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:32" s="13" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="12" t="s">
         <v>324</v>
       </c>
@@ -5992,7 +6024,7 @@
       <c r="AE133" s="3"/>
       <c r="AF133" s="3"/>
     </row>
-    <row r="134" spans="1:32" s="13" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:32" s="13" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="s">
         <v>324</v>
       </c>
@@ -6068,7 +6100,7 @@
       <c r="AE134" s="3"/>
       <c r="AF134" s="3"/>
     </row>
-    <row r="135" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>223</v>
       </c>
@@ -6102,7 +6134,7 @@
       <c r="AE135" s="3"/>
       <c r="AF135" s="3"/>
     </row>
-    <row r="136" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>274</v>
       </c>
@@ -6116,7 +6148,7 @@
         <v>274</v>
       </c>
       <c r="E136" s="5">
-        <v>295</v>
+        <v>250</v>
       </c>
       <c r="J136" s="5">
         <v>340</v>
@@ -6145,7 +6177,7 @@
       <c r="AE136" s="3"/>
       <c r="AF136" s="3"/>
     </row>
-    <row r="137" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>274</v>
       </c>
@@ -6159,7 +6191,7 @@
         <v>277</v>
       </c>
       <c r="E137" s="5">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="J137" s="5">
         <v>340</v>
@@ -6188,7 +6220,7 @@
       <c r="AE137" s="3"/>
       <c r="AF137" s="3"/>
     </row>
-    <row r="138" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>274</v>
       </c>
@@ -6219,7 +6251,7 @@
       <c r="AE138" s="3"/>
       <c r="AF138" s="3"/>
     </row>
-    <row r="139" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>280</v>
       </c>
@@ -6256,7 +6288,7 @@
       <c r="AE139" s="3"/>
       <c r="AF139" s="3"/>
     </row>
-    <row r="140" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>283</v>
       </c>
@@ -6293,7 +6325,7 @@
       <c r="AE140" s="3"/>
       <c r="AF140" s="3"/>
     </row>
-    <row r="141" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>15</v>
       </c>
@@ -6336,7 +6368,7 @@
       <c r="AE141" s="3"/>
       <c r="AF141" s="3"/>
     </row>
-    <row r="142" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>15</v>
       </c>
@@ -6382,7 +6414,7 @@
       <c r="AE142" s="3"/>
       <c r="AF142" s="3"/>
     </row>
-    <row r="143" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>15</v>
       </c>
@@ -6419,7 +6451,7 @@
       <c r="AE143" s="3"/>
       <c r="AF143" s="3"/>
     </row>
-    <row r="144" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>15</v>
       </c>
@@ -6468,7 +6500,7 @@
       <c r="AE144" s="3"/>
       <c r="AF144" s="3"/>
     </row>
-    <row r="145" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>15</v>
       </c>
@@ -6508,7 +6540,7 @@
       <c r="AE145" s="3"/>
       <c r="AF145" s="3"/>
     </row>
-    <row r="146" spans="1:32" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:32" s="4" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>15</v>
       </c>
@@ -6551,7 +6583,7 @@
       <c r="AE146" s="3"/>
       <c r="AF146" s="3"/>
     </row>
-    <row r="147" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>15</v>
       </c>
@@ -6591,7 +6623,7 @@
       <c r="AE147" s="3"/>
       <c r="AF147" s="3"/>
     </row>
-    <row r="148" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>15</v>
       </c>
@@ -6622,7 +6654,7 @@
       <c r="AE148" s="3"/>
       <c r="AF148" s="3"/>
     </row>
-    <row r="149" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>300</v>
       </c>
@@ -6653,7 +6685,7 @@
       <c r="AE149" s="3"/>
       <c r="AF149" s="3"/>
     </row>
-    <row r="150" spans="1:32" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:32" s="4" customFormat="1" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>64</v>
       </c>
@@ -6667,19 +6699,19 @@
         <v>303</v>
       </c>
       <c r="E150" s="5">
-        <v>358</v>
+        <v>130</v>
       </c>
       <c r="F150" s="8">
-        <v>308.2</v>
-      </c>
-      <c r="H150" s="4">
-        <v>413.4</v>
+        <v>290</v>
+      </c>
+      <c r="H150" s="8">
+        <v>290</v>
       </c>
       <c r="J150" s="8">
         <v>100</v>
       </c>
       <c r="L150" s="8">
-        <v>308.2</v>
+        <v>290</v>
       </c>
       <c r="N150" s="5">
         <v>83</v>
@@ -6702,7 +6734,7 @@
       <c r="AE150" s="3"/>
       <c r="AF150" s="3"/>
     </row>
-    <row r="151" spans="1:32" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:32" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>304</v>
       </c>
@@ -6751,7 +6783,7 @@
       <c r="AE151" s="3"/>
       <c r="AF151" s="3"/>
     </row>
-    <row r="152" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:32" s="13" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="12" t="s">
         <v>307</v>
       </c>
@@ -6803,7 +6835,7 @@
       <c r="AE152" s="3"/>
       <c r="AF152" s="3"/>
     </row>
-    <row r="153" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:32" s="13" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="12" t="s">
         <v>223</v>
       </c>
@@ -6834,7 +6866,7 @@
       <c r="AE153" s="3"/>
       <c r="AF153" s="3"/>
     </row>
-    <row r="154" spans="1:32" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:32" s="13" customFormat="1" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="12" t="s">
         <v>311</v>
       </c>
@@ -6874,7 +6906,7 @@
       <c r="AE154" s="3"/>
       <c r="AF154" s="3"/>
     </row>
-    <row r="155" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:32" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>280</v>
       </c>
@@ -6897,8 +6929,979 @@
         <v>283</v>
       </c>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:32" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="157" spans="1:32" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="158" spans="1:32" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="159" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="P159" s="15"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AF159" xr:uid="{26C02D22-C5E3-6846-A49B-8DFDD4C89904}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Deep orange fruits"/>
+        <filter val="Deep orange fruits "/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E110092-D6C3-6D4D-A67C-BB13067E22A0}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E159"/>
+  <sheetViews>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152:A154"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="68" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="85" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A122" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A133" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A136" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A140" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A149" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A152" s="12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A154" s="12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" ht="51" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="158" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="159" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F3BED0-0C51-444B-852D-A1A9EC672885}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>311</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>